<commit_message>
not admitted works in rating
</commit_message>
<xml_diff>
--- a/uploads/rating.xlsx
+++ b/uploads/rating.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -414,7 +414,7 @@
         <v>—</v>
       </c>
       <c r="C2" t="str">
-        <v>Моя прекрасная работа</v>
+        <v>Права человека</v>
       </c>
       <c r="D2" t="str">
         <v>исследования в области гуманитарных наук и права</v>
@@ -429,38 +429,12 @@
         <v>МОАУ Лицей 4</v>
       </c>
       <c r="H2">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>—</v>
-      </c>
-      <c r="B3" t="str">
-        <v>—</v>
-      </c>
-      <c r="C3" t="str">
-        <v>Еще одна работа</v>
-      </c>
-      <c r="D3" t="str">
-        <v>исследования в области гуманитарных наук и права</v>
-      </c>
-      <c r="E3" t="str">
-        <v>Демидов Василий Иванович</v>
-      </c>
-      <c r="F3" t="str">
-        <v>Доктор/Профессор</v>
-      </c>
-      <c r="G3" t="str">
-        <v>МОАУ Лицей 4</v>
-      </c>
-      <c r="H3">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>